<commit_message>
update auto retry hours
</commit_message>
<xml_diff>
--- a/Traveloka_DataAutomation_Performer_Portal/Data/Config.xlsx
+++ b/Traveloka_DataAutomation_Performer_Portal/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kalyana\Traveloka_DataAutomation_Performer_Portal\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kalyana\dataautomation_personal\Traveloka_DataAutomation_Performer_Portal\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8B4CFB3-9CD4-4C2C-B7DF-B9F067A1B4E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DB524B2-1B57-4798-A5E5-802E390ECA07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3552" yWindow="1236" windowWidth="17280" windowHeight="9000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="28992" windowHeight="14736" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="61">
   <si>
     <t>Name</t>
   </si>
@@ -196,6 +196,18 @@
   </si>
   <si>
     <t>AutoRetryPostpone</t>
+  </si>
+  <si>
+    <t>AutoRetryMaxDay</t>
+  </si>
+  <si>
+    <t>RPA_Moon_AutoRetryMaxDay</t>
+  </si>
+  <si>
+    <t>AutoRetrySchedule</t>
+  </si>
+  <si>
+    <t>RPA_Moon_AutoRetrySchedule</t>
   </si>
 </sst>
 </file>
@@ -275,9 +287,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -315,7 +327,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -421,7 +433,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -563,7 +575,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2829,10 +2841,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A4" sqref="A4:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.375" defaultRowHeight="14.95" customHeight="1"/>
@@ -2911,8 +2923,22 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.3" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.3" customHeight="1"/>
+    <row r="6" spans="1:26" ht="14.3" customHeight="1">
+      <c r="A6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="14.3" customHeight="1">
+      <c r="A7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" t="s">
+        <v>60</v>
+      </c>
+    </row>
     <row r="8" spans="1:26" ht="14.3" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.3" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.3" customHeight="1"/>
@@ -3904,8 +3930,6 @@
     <row r="996" ht="14.3" customHeight="1"/>
     <row r="997" ht="14.3" customHeight="1"/>
     <row r="998" ht="14.3" customHeight="1"/>
-    <row r="999" ht="14.3" customHeight="1"/>
-    <row r="1000" ht="14.3" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>